<commit_message>
finally got the calendar in the right repo
</commit_message>
<xml_diff>
--- a/calendar.xlsx
+++ b/calendar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grinco-my.sharepoint.com/personal/wordenea_grinnell_edu/Documents/Desktop/Year 3 Sem 2/CSC324/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{B8926844-8B46-4D91-942F-6FB6A6B14CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F98A5D0A-C14C-4161-A87B-8F9DB86C7BEE}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="8_{B8926844-8B46-4D91-942F-6FB6A6B14CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D752400-32A6-45BD-8395-57F72C588795}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17304" windowHeight="9144" xr2:uid="{C930A5AA-25AA-46F3-9B4F-C2B0AF55FD1A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C930A5AA-25AA-46F3-9B4F-C2B0AF55FD1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
   <si>
     <t>M</t>
   </si>
@@ -100,7 +100,7 @@
     <t>L means lab</t>
   </si>
   <si>
-    <t>Rest of time is typically class</t>
+    <t>Rest of time is typically class or general HW time</t>
   </si>
 </sst>
 </file>
@@ -116,12 +116,54 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -136,8 +178,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E742B3-1BA7-4888-902F-28AF44697F1D}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,16 +537,16 @@
       <c r="A2">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3">
         <v>341</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3">
         <v>341</v>
       </c>
     </row>
@@ -504,88 +554,94 @@
       <c r="A3">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3">
         <v>341</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3">
         <v>341</v>
       </c>
-      <c r="F3">
-        <v>324</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="F3" s="6">
+        <v>324</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H3" t="s">
-        <v>17</v>
+      <c r="H3" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>499</v>
       </c>
-      <c r="F4">
-        <v>324</v>
-      </c>
-      <c r="G4">
+      <c r="F4" s="6">
+        <v>324</v>
+      </c>
+      <c r="G4" s="4">
         <v>499</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4">
         <v>499</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -593,22 +649,25 @@
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="8">
         <v>499</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
         <v>499</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>499</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="4">
         <v>499</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G7" s="4">
+        <v>499</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -616,22 +675,25 @@
       <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8">
-        <v>324</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="6">
+        <v>324</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D8">
-        <v>324</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="6">
+        <v>324</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F8">
-        <v>324</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="F8" s="6">
+        <v>324</v>
+      </c>
+      <c r="G8" s="4">
+        <v>499</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -639,25 +701,25 @@
       <c r="A9">
         <v>3</v>
       </c>
-      <c r="B9">
-        <v>324</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" s="6">
+        <v>324</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D9">
-        <v>324</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="D9" s="6">
+        <v>324</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F9">
-        <v>324</v>
-      </c>
-      <c r="G9">
-        <v>324</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="F9" s="6">
+        <v>324</v>
+      </c>
+      <c r="G9" s="6">
+        <v>324</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -665,25 +727,21 @@
       <c r="A10">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D10">
-        <v>324</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D10" s="6">
+        <v>324</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -691,39 +749,40 @@
       <c r="A11">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D11">
-        <v>324</v>
-      </c>
-      <c r="F11" t="s">
-        <v>7</v>
-      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6">
+        <v>324</v>
+      </c>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -731,16 +790,19 @@
       <c r="A13">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H13" t="s">
+      <c r="G13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -748,16 +810,19 @@
       <c r="A14">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -765,13 +830,16 @@
       <c r="A15">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>